<commit_message>
Prolog black box and test suite done
</commit_message>
<xml_diff>
--- a/test_plan.xlsx
+++ b/test_plan.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aae8df57aa70805f/mru/comp3649/proj/comp3649project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="237" documentId="8_{3AB129F9-6C21-034E-B68D-3118804A730C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E26BDDD-79F6-E54E-8321-27AF78B47A76}"/>
+  <xr:revisionPtr revIDLastSave="289" documentId="8_{3AB129F9-6C21-034E-B68D-3118804A730C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A429E228-FFE5-BF4D-B0B3-A85C605ABB50}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{648EA1FE-8C1C-FB4A-A645-0D83DAA06A0B}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" activeTab="1" xr2:uid="{648EA1FE-8C1C-FB4A-A645-0D83DAA06A0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Python" sheetId="1" r:id="rId1"/>
+    <sheet name="Prolog" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Prolog!$A$1:$I$18</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="90">
-  <si>
-    <t>Test Plan</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="117">
   <si>
     <t>#</t>
   </si>
@@ -397,9 +398,6 @@
     <t>Slowest test to run. Since we know it fails, all permuations are checked for each of the 20 semesters</t>
   </si>
   <si>
-    <t>test jsons stored in `data/input/test/`</t>
-  </si>
-  <si>
     <t>Some issues using the newer courses to get different options, since our source CSV had no info so the searches failed.</t>
   </si>
   <si>
@@ -432,6 +430,186 @@
     <t>Degree successfully scheduled in 5.0 years (10 semesters)
 num_semesters: 10
 num_years: 5.0</t>
+  </si>
+  <si>
+    <t>Python Test Plan</t>
+  </si>
+  <si>
+    <t>Prolog Test Plan</t>
+  </si>
+  <si>
+    <t>prolog test jsons stored in `data/input/test/prolog/`</t>
+  </si>
+  <si>
+    <t>python test jsons stored in `data/input/test/python`</t>
+  </si>
+  <si>
+    <t>While we were thinking "pass", we realize that in this implementation, having a full degree means that no possible schedule can be generated. It is acceptable to us that this results in a fail case. So we will mark this test as a pass.</t>
+  </si>
+  <si>
+    <t>semesters = 0</t>
+  </si>
+  <si>
+    <t>courses_for_semester = 0</t>
+  </si>
+  <si>
+    <t>courses_for_semester = -1</t>
+  </si>
+  <si>
+    <t>taken = []
+semesters = 8
+courses_for_semester = 5</t>
+  </si>
+  <si>
+    <t>taken =  [
+                "COMP1631",
+                "MATH1200",
+                "COMP1633",
+                "PHIL1179"
+        ]</t>
+  </si>
+  <si>
+    <t>taken =  [
+                "COMP1631",
+                "MATH1200",
+                "COMP1633",
+                "PHIL1179",
+                "COMP2631",
+                "MATH1271",
+                "COMP2655",
+                "COMP2633"
+        ]</t>
+  </si>
+  <si>
+    <t>taken =  [
+                "COMP1631",
+                "MATH1200",
+                "COMP1633",
+                "PHIL1179",
+                "COMP2631",
+                "MATH1271",
+                "COMP2655",
+                "COMP2633",
+                "COMP2613",
+                "COMP2659",
+                "COMP3649",
+                "MATH2234"
+        ]</t>
+  </si>
+  <si>
+    <t>semesters = -1</t>
+  </si>
+  <si>
+    <t>years_to_grad = -1</t>
+  </si>
+  <si>
+    <t>taken = []
+semesters = 2
+courses_for_semester = 1</t>
+  </si>
+  <si>
+    <t>taken = []
+semesters = 4
+courses_for_semester = 3</t>
+  </si>
+  <si>
+    <t>taken = []
+semesters = 6
+courses_for_semester = 4</t>
+  </si>
+  <si>
+    <t>taken = []
+semesters = 20
+courses_for_semester = 10</t>
+  </si>
+  <si>
+    <t>taken = []
+semesters = 16
+courses_for_semester = 5</t>
+  </si>
+  <si>
+    <t>no taken, no options/cognate
+(16 courses)
+semesters = 32
+courses_for_semester = 1</t>
+  </si>
+  <si>
+    <t>The provided file did not generate a plan</t>
+  </si>
+  <si>
+    <t>0,winter,phil1179,mon/16/mru,wed/16/mru,fri/16/mru,
+0,winter,comp3309,tue/11/mru,thu/11/mru,thu/10/mru,
+1,fall,comp1631,mon/11/mru,wed/11/mru,fri/11/mru,
+1,fall,math1200,tue/13/mru,thu/13/mru,thu/12/mru,
+1,fall,math1203,mon/16/mru,wed/16/mru,fri/16/mru,
+2,winter,comp1633,mon/4/mru,wed/4/mru,fri/4/mru,
+2,winter,math1271,mon/8/mru,wed/8/mru,fri/8/mru,
+2,winter,math2234,mon/10/mru,wed/10/mru,fri/10/mru,
+3,fall,comp2631,tue/10/mru,thu/10/mru,thu/9/mru,
+3,fall,comp2613,tue/14/mru,thu/14/mru,thu/13/mru,
+3,fall,comp2655,mon/14/mru,wed/14/mru,fri/14/mru,
+4,winter,comp2659,mon/15/mru,wed/15/mru,fri/15/mru,
+4,winter,comp2633,tue/8/mru,thu/8/mru,thu/7/mru,
+4,winter,comp3614,tue/14/mru,tue/15/mru,thu/14/mru,
+4,winter,comp3649,tue/16/mru,thu/16/mru,thu/15/mru,
+5,fall,comp3659,mon/8/mru,wed/8/mru,fri/8/mru,</t>
+  </si>
+  <si>
+    <t>0,winter,comp3309,tue/11/mru,thu/11/mru,thu/10/mru,
+0,winter,math2234,mon/10/mru,wed/10/mru,fri/10/mru,
+1,fall,comp2631,tue/10/mru,thu/10/mru,thu/9/mru,
+1,fall,comp2655,mon/14/mru,wed/14/mru,fri/14/mru,
+1,fall,math1203,mon/16/mru,wed/16/mru,fri/16/mru,
+2,winter,comp2659,mon/15/mru,wed/15/mru,fri/15/mru,
+2,winter,math1271,mon/8/mru,wed/8/mru,fri/8/mru,
+2,winter,comp2633,tue/8/mru,thu/8/mru,thu/7/mru,
+3,fall,comp2613,tue/14/mru,thu/14/mru,thu/13/mru,
+3,fall,comp3659,mon/8/mru,wed/8/mru,fri/8/mru,
+4,winter,comp3614,tue/14/mru,tue/15/mru,thu/14/mru,
+4,winter,comp3649,tue/16/mru,thu/16/mru,thu/15/mru,</t>
+  </si>
+  <si>
+    <t>0,winter,comp2659,mon/15/mru,wed/15/mru,fri/15/mru,
+0,winter,comp3309,tue/11/mru,thu/11/mru,thu/10/mru,
+0,winter,math2234,mon/10/mru,wed/10/mru,fri/10/mru,
+1,fall,comp2613,tue/14/mru,thu/14/mru,thu/13/mru,
+1,fall,math1203,mon/16/mru,wed/16/mru,fri/16/mru,
+1,fall,comp3659,mon/8/mru,wed/8/mru,fri/8/mru,
+2,winter,comp3614,tue/14/mru,tue/15/mru,thu/14/mru,
+2,winter,comp3649,tue/16/mru,thu/16/mru,thu/15/mru,</t>
+  </si>
+  <si>
+    <t>pass in &lt; 6 sem</t>
+  </si>
+  <si>
+    <t>pass in &lt; 4 sem</t>
+  </si>
+  <si>
+    <t>pass in &lt; 2 sem</t>
+  </si>
+  <si>
+    <t>0,winter,comp3309,tue/11/mru,thu/11/mru,thu/10/mru,
+0,winter,comp3614,tue/14/mru,tue/15/mru,thu/14/mru,
+1,fall,math1203,mon/16/mru,wed/16/mru,fri/16/mru,
+1,fall,comp3659,mon/8/mru,wed/8/mru,fri/8/mru,</t>
+  </si>
+  <si>
+    <t>1,fall,comp1631,mon/11/mru,wed/11/mru,fri/11/mru,
+2,winter,comp1633,mon/10/mru,wed/10/mru,fri/10/mru,
+3,fall,comp2631,tue/10/mru,thu/10/mru,thu/9/mru,
+5,fall,comp2655,mon/14/mru,wed/14/mru,fri/14/mru,
+7,fall,math1200,tue/13/mru,thu/13/mru,thu/12/mru,
+9,fall,math1203,mon/16/mru,wed/16/mru,fri/16/mru,
+10,winter,math1271,mon/8/mru,wed/8/mru,fri/8/mru,
+11,fall,comp2613,tue/14/mru,thu/14/mru,thu/13/mru,
+12,winter,phil1179,mon/16/mru,wed/16/mru,fri/16/mru,
+14,winter,comp2659,mon/15/mru,wed/15/mru,fri/15/mru,
+16,winter,comp2633,tue/8/mru,thu/8/mru,thu/7/mru,
+17,fall,comp3309,tue/10/mru,thu/10/mru,thu/9/mru,
+18,winter,comp3614,tue/14/mru,tue/15/mru,thu/14/mru,
+20,winter,comp3649,tue/16/mru,thu/16/mru,thu/15/mru,
+21,fall,comp3659,mon/8/mru,wed/8/mru,fri/8/mru,
+22,winter,math2234,mon/10/mru,wed/10/mru,fri/10/mru,</t>
   </si>
 </sst>
 </file>
@@ -561,7 +739,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -894,11 +1092,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15EE35DF-1E31-B34F-BCFF-1FD3BCC0EA75}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -918,10 +1116,10 @@
     <row r="1" spans="1:9" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.35">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -931,31 +1129,31 @@
     </row>
     <row r="3" spans="1:9" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>4</v>
-      </c>
       <c r="H3" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -963,26 +1161,26 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="str">
         <f>CONCATENATE(A4,".json")</f>
         <v>1.json</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -990,26 +1188,26 @@
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="str">
         <f t="shared" ref="D5:D30" si="0">CONCATENATE(A5,".json")</f>
         <v>2.json</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1017,26 +1215,26 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>3.json</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1044,26 +1242,26 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4.json</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>4.json</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1071,26 +1269,26 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>5.json</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>5.json</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1098,26 +1296,26 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>6.json</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1125,26 +1323,26 @@
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>7.json</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -1152,26 +1350,26 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>8.json</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1179,26 +1377,26 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>9.json</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>9.json</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1206,26 +1404,26 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>10.json</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -1233,26 +1431,26 @@
         <v>11</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>11.json</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="170" x14ac:dyDescent="0.2">
@@ -1260,26 +1458,26 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>12.json</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="238" x14ac:dyDescent="0.2">
@@ -1287,26 +1485,26 @@
         <v>13</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>13.json</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>13.json</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -1314,26 +1512,26 @@
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>14.json</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -1341,29 +1539,29 @@
         <v>15</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>15.json</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -1371,29 +1569,29 @@
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>16.json</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="D19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>16.json</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="170" x14ac:dyDescent="0.2">
@@ -1401,26 +1599,26 @@
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>17.json</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -1428,26 +1626,26 @@
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>18.json</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="306" x14ac:dyDescent="0.2">
@@ -1455,26 +1653,26 @@
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>19.json</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="170" x14ac:dyDescent="0.2">
@@ -1482,29 +1680,29 @@
         <v>20</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>20.json</v>
       </c>
       <c r="E23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="F23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="H23" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="119" x14ac:dyDescent="0.2">
@@ -1512,26 +1710,26 @@
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>21.json</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="H24" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -1539,29 +1737,29 @@
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="D25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>22.json</v>
       </c>
       <c r="E25" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1569,26 +1767,515 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>23.json</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="G26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="I3 H1:H1048576">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",H1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",H1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0408BD7-DCFB-044D-9C76-99080A8D7D40}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="69.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.35">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>CONCATENATE(A4,".json")</f>
+        <v>1.json</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f t="shared" ref="D5:D18" si="0">CONCATENATE(A5,".json")</f>
+        <v>2.json</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>3.json</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>4.json</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>5.json</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>6.json</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>7.json</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>8.json</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>9.json</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>10.json</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="204" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>11.json</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>12.json</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>13.json</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>23</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="2" t="str">
-        <f t="shared" si="0"/>
+      <c r="C17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f>CONCATENATE(A17,".json")</f>
         <v>23.json</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="F17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>22</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>22.json</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>58</v>
+      <c r="G18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prolog and Python tests green. Cleaned up Python.
</commit_message>
<xml_diff>
--- a/test_plan.xlsx
+++ b/test_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aae8df57aa70805f/mru/comp3649/proj/comp3649project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="306" documentId="8_{3AB129F9-6C21-034E-B68D-3118804A730C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE2F7F76-6B18-674B-AFA0-21DD3FB75109}"/>
+  <xr:revisionPtr revIDLastSave="398" documentId="8_{3AB129F9-6C21-034E-B68D-3118804A730C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FFCAE73-9D12-7A4C-93C1-2D61E6FBC2B8}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" activeTab="1" xr2:uid="{648EA1FE-8C1C-FB4A-A645-0D83DAA06A0B}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Prolog" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Prolog!$A$1:$I$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Prolog!$A$1:$I$26</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="149">
   <si>
     <t>#</t>
   </si>
@@ -665,6 +665,176 @@
                 "comp5690",
                 "comp4630"
         ],</t>
+  </si>
+  <si>
+    <t>Junior Options
+No senior</t>
+  </si>
+  <si>
+    <t>In prolog we check for all valid junior/senior options before execution. They both must be valid and included.</t>
+  </si>
+  <si>
+    <t>Invalid Junior options</t>
+  </si>
+  <si>
+    <t>Invalid Senior options</t>
+  </si>
+  <si>
+    <t>Invalid Junior and Senior options</t>
+  </si>
+  <si>
+    <t>option test,
+invalid names</t>
+  </si>
+  <si>
+    <t>option test,
+invalid number of arguments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "jun": [
+                "comp3533",
+                "comp1234",
+                "math1234"
+        ],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "sen": [
+                "gned0101",
+                "cmpo2001",
+                "marc1000"
+        ],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "jun": [
+                "comp3533",
+                "comp1234",
+                "math1234"
+        ],
+        "sen": [
+                "gned0101",
+                "cmpo2001",
+                "marc1000"
+        ],</t>
+  </si>
+  <si>
+    <t>Invalid Cognate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "chosen_jun_options": [
+                "comp1",
+                "math",
+                "marc101"
+        ],</t>
+  </si>
+  <si>
+    <t>0,winter,comp1631,mon/11/mru,wed/11/mru,fri/11/mru,
+  0,winter,math1200,tue/13/mru,thu/13/mru,thu/12/mru,
+  0,winter,math1203,mon/16/mru,wed/16/mru,fri/16/mru,
+  0,winter,phil1179,mon/8/mru,wed/8/mru,fri/8/mru,
+  0,winter,comp3309,tue/10/mru,thu/10/mru,thu/9/mru,
+  1,fall,comp1633,mon/4/mru,wed/4/mru,fri/4/mru,
+  1,fall,comp2521,tue/315/mru,thu/315/mru,thu/314/mru,
+  1,fall,math1271,mon/8/mru,wed/8/mru,fri/8/mru,
+  1,fall,math2234,mon/2/mru,wed/2/mru,fri/2/mru,
+  2,winter,comp2613,tue/14/mru,thu/14/mru,thu/13/mru,
+  2,winter,comp2631,tue/10/mru,thu/10/mru,thu/9/mru,
+  2,winter,comp2655,mon/14/mru,wed/14/mru,fri/14/mru,
+  2,winter,comp4522,mon/1110/mru,wed/1110/mru,fri/1110/mru,
+  3,fall,comp2633,tue/2/mru,thu/2/mru,thu/1/mru,
+  3,fall,comp3533,mon/510/mru,wed/510/mru,fri/510/mru,
+  3,fall,comp3614,tue/14/mru,tue/15/mru,thu/14/mru,
+  3,fall,comp3625,tue/620/mru,tue/621/mru,thu/620/mru,
+  3,fall,comp3649,tue/10/mru,thu/10/mru,thu/9/mru,
+  4,winter,comp2659,mon/15/mru,wed/15/mru,fri/15/mru,
+  4,winter,comp4630,mon/2011/mru,wed/2011/mru,fri/2011/mru,
+  4,winter,comp4635,tue/17/mru,tue/18/mru,tue/19/mru,
+  5,fall,comp3659,mon/8/mru,wed/8/mru,fri/8/mru,</t>
+  </si>
+  <si>
+    <t>0,winter,comp5690,any/17/mru,any/18/mru,any/19/mru,
+  0,winter,comp1631,mon/11/mru,wed/11/mru,fri/11/mru,
+  0,winter,math1200,tue/13/mru,thu/13/mru,thu/12/mru,
+  0,winter,math1203,mon/16/mru,wed/16/mru,fri/16/mru,
+  0,winter,phil1179,mon/8/mru,wed/8/mru,fri/8/mru,
+  1,fall,comp1633,mon/4/mru,wed/4/mru,fri/4/mru,
+  1,fall,comp2521,tue/315/mru,thu/315/mru,thu/314/mru,
+  1,fall,comp3309,tue/10/mru,thu/10/mru,thu/9/mru,
+  1,fall,math1271,mon/8/mru,wed/8/mru,fri/8/mru,
+  1,fall,math2234,mon/2/mru,wed/2/mru,fri/2/mru,
+  2,winter,comp2613,tue/14/mru,thu/14/mru,thu/13/mru,
+  2,winter,comp2631,tue/10/mru,thu/10/mru,thu/9/mru,
+  2,winter,comp2655,mon/14/mru,wed/14/mru,fri/14/mru,
+  3,fall,comp2633,tue/2/mru,thu/2/mru,thu/1/mru,
+  3,fall,comp3533,mon/510/mru,wed/510/mru,fri/510/mru,
+  3,fall,comp3614,tue/14/mru,tue/15/mru,thu/14/mru,
+  3,fall,comp3625,tue/620/mru,tue/621/mru,thu/620/mru,
+  3,fall,comp3649,tue/10/mru,thu/10/mru,thu/9/mru,
+  4,winter,comp2659,mon/15/mru,wed/15/mru,fri/15/mru,
+  4,winter,comp4630,mon/2011/mru,wed/2011/mru,fri/2011/mru,
+  5,fall,comp3659,mon/8/mru,wed/8/mru,fri/8/mru,
+  5,fall,comp4555,mon/810/mru,wed/810/mru,fri/810/mru,</t>
+  </si>
+  <si>
+    <t>Invalid Course:  comp1234  in make_graph
+Invalid Course:  comp3533  in make_graph
+Invalid Course:  math1234  in make_graph
+Degree was not able to be scheduled in 4 years</t>
+  </si>
+  <si>
+    <t>Invalid Course:  cmpo2001  in make_graph
+Invalid Course:  gned0101  in make_graph
+Invalid Course:  marc1000  in make_graph
+Degree was not able to be scheduled in 4 years</t>
+  </si>
+  <si>
+    <t>Invalid Course:  BAR  in make_graph
+Invalid Course:  FIZZBUZZ  in make_graph
+Invalid Course:  FOO  in make_graph
+Invalid Course:  FOOBAR  in make_graph
+Degree was not able to be scheduled in 4 years</t>
+  </si>
+  <si>
+    <t>Invalid Course:  BAR  in make_graph
+Invalid Course:  FIZZBUZZ  in make_graph
+Invalid Course:  FOO  in make_graph
+Invalid Course:  FOOBAR  in make_graph
+Invalid Course:  cmpo2001  in make_graph
+Invalid Course:  comp1234  in make_graph
+Invalid Course:  comp3533  in make_graph
+Invalid Course:  gned0101  in make_graph
+Invalid Course:  marc1000  in make_graph
+Invalid Course:  math1234  in make_graph
+Degree was not able to be scheduled in 4 years</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "chosen_sen_options": [
+                "gned0101",
+                "cmpo2001",
+                "marc1000"
+        ],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "cognate_choice": [
+                "FOO",
+                "BAR",
+                "FOOBAR",
+                "FIZZBUZZ"
+        ],</t>
+  </si>
+  <si>
+    <t>all of 24-26</t>
+  </si>
+  <si>
+    <t>*note that test # might be different than order ran from tests.pl</t>
+  </si>
+  <si>
+    <t>*note that test # might be different than order ran from run_tests.py</t>
+  </si>
+  <si>
+    <t>run tests (from root folder/parent folder of run_tests.py): "python3 run_tests.py"</t>
+  </si>
+  <si>
+    <t>run tests (from prolog folder): "swipl tests.pl" -&gt; "run_tests."</t>
   </si>
 </sst>
 </file>
@@ -754,7 +924,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -788,6 +958,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1165,13 +1338,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15EE35DF-1E31-B34F-BCFF-1FD3BCC0EA75}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD22"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1196,84 +1369,68 @@
       <c r="D1" s="10" t="s">
         <v>91</v>
       </c>
+      <c r="G1" s="15" t="s">
+        <v>147</v>
+      </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+    <row r="2" spans="1:9" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="G2" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I4" s="14" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f>CONCATENATE(A4,".json")</f>
-        <v>1.json</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f t="shared" ref="D5:D30" si="0">CONCATENATE(A5,".json")</f>
-        <v>2.json</v>
+        <f>CONCATENATE(A5,".json")</f>
+        <v>1.json</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>9</v>
@@ -1281,26 +1438,26 @@
       <c r="G5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.json</v>
+        <f t="shared" ref="D6:D31" si="0">CONCATENATE(A6,".json")</f>
+        <v>2.json</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>101</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
@@ -1314,20 +1471,20 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>4.json</v>
+        <v>3.json</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>9</v>
@@ -1339,28 +1496,28 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>5.json</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>14</v>
+        <v>4.json</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>57</v>
@@ -1368,20 +1525,20 @@
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>6.json</v>
+        <v>5.json</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>9</v>
@@ -1395,74 +1552,74 @@
     </row>
     <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>7.json</v>
+        <v>6.json</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>7.json</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="H11" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>8.json</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>9.json</v>
+        <v>8.json</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>17</v>
@@ -1476,20 +1633,20 @@
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>10.json</v>
+        <v>9.json</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>17</v>
@@ -1501,109 +1658,109 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>10.json</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11.json</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="170" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>12.json</v>
+        <v>11.json</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="170" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="0"/>
+        <v>12.json</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>13.json</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>14.json</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>57</v>
@@ -1611,47 +1768,44 @@
     </row>
     <row r="18" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>15.json</v>
+        <v>14.json</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>81</v>
+        <v>60</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>16.json</v>
+        <v>15.json</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>63</v>
@@ -1660,212 +1814,350 @@
         <v>9</v>
       </c>
       <c r="G19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>16.json</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" s="3" t="s">
+      <c r="H20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="170" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+    <row r="21" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>17</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="2" t="str">
+      <c r="D21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>17.json</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>18.json</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="306" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>19.json</v>
+        <v>18.json</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="306" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>20.json</v>
+        <v>19.json</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:9" ht="170" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>21.json</v>
+        <v>20.json</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>21.json</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="H25" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <v>22</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="2" t="str">
+      <c r="D26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>22.json</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I25" s="3" t="s">
+      <c r="H26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="2" t="str">
+      <c r="D27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>23.json</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H27" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>24</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>24.json</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>25</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>25.json</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>26</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>26.json</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>27</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="2" t="str">
+        <f t="shared" ref="D31" si="1">CONCATENATE(A31,".json")</f>
+        <v>27.json</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I3 H1:H1048576">
+  <conditionalFormatting sqref="I4 H1:H1048576">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",H1)))</formula>
     </cfRule>
@@ -1879,13 +2171,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0408BD7-DCFB-044D-9C76-99080A8D7D40}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1910,84 +2202,67 @@
       <c r="D1" s="10" t="s">
         <v>90</v>
       </c>
+      <c r="G1" s="15" t="s">
+        <v>148</v>
+      </c>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="B2" s="2"/>
+      <c r="G2" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I4" s="14" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f>CONCATENATE(A4,".json")</f>
-        <v>1.json</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f t="shared" ref="D5:D22" si="0">CONCATENATE(A5,".json")</f>
-        <v>2.json</v>
+        <f>CONCATENATE(A5,".json")</f>
+        <v>1.json</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>9</v>
@@ -1995,26 +2270,26 @@
       <c r="G5" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="7" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>3.json</v>
+        <f t="shared" ref="D6:D26" si="0">CONCATENATE(A6,".json")</f>
+        <v>2.json</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
@@ -2028,20 +2303,20 @@
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>4.json</v>
+        <v>3.json</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>9</v>
@@ -2053,22 +2328,22 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>5.json</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>102</v>
+        <v>4.json</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>9</v>
@@ -2082,20 +2357,20 @@
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>6.json</v>
+        <v>5.json</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>9</v>
@@ -2109,20 +2384,20 @@
     </row>
     <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>7.json</v>
+        <v>6.json</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>9</v>
@@ -2134,28 +2409,28 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>8.json</v>
+        <v>7.json</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>109</v>
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>57</v>
@@ -2163,20 +2438,20 @@
     </row>
     <row r="12" spans="1:9" ht="272" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>9.json</v>
+        <v>8.json</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>17</v>
@@ -2190,20 +2465,20 @@
     </row>
     <row r="13" spans="1:9" ht="272" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>10.json</v>
+        <v>9.json</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>17</v>
@@ -2215,271 +2490,392 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="204" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="272" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>10.json</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="204" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>11.json</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="170" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>12.json</v>
+        <v>11.json</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="170" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="0"/>
+        <v>12.json</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="238" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f t="shared" si="0"/>
         <v>13.json</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>14.json</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="3"/>
       <c r="H17" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>124</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>15.json</v>
+        <v>14.json</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="H18" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="119" x14ac:dyDescent="0.2">
+      <c r="I18" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>16.json</v>
+        <v>15.json</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="H19" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="119" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>16.json</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="372" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>17</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>17.json</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="170" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>118</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="2" t="str">
-        <f t="shared" ref="D21" si="1">CONCATENATE(A21,".json")</f>
-        <v>18.json</v>
+        <f t="shared" si="0"/>
+        <v>17.json</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>136</v>
+      </c>
       <c r="H21" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="372" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
+        <v>18</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="2" t="str">
+        <f t="shared" ref="D22:D25" si="1">CONCATENATE(A22,".json")</f>
+        <v>18.json</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>19</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>19.json</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>20</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>20.json</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="170" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>21</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>21.json</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="272" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <v>22</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="2" t="str">
+      <c r="D26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>22.json</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="H26" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="2" t="str">
-        <f>CONCATENATE(A23,".json")</f>
+      <c r="D27" s="2" t="str">
+        <f>CONCATENATE(A27,".json")</f>
         <v>23.json</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I23" s="3" t="s">
+      <c r="H27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I3 H1:H16 H22:H1048576">
+  <conditionalFormatting sqref="I4 H1:H17 H26:H1048576">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",H1)))</formula>
     </cfRule>
@@ -2487,12 +2883,12 @@
       <formula>NOT(ISERROR(SEARCH("N",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17:H21">
+  <conditionalFormatting sqref="H18:H25">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",H17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Y",H18)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",H17)))</formula>
+      <formula>NOT(ISERROR(SEARCH("N",H18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
run_tests.py->unit tests. Refactored can_schedule
</commit_message>
<xml_diff>
--- a/test_plan.xlsx
+++ b/test_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aae8df57aa70805f/mru/comp3649/proj/comp3649project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="398" documentId="8_{3AB129F9-6C21-034E-B68D-3118804A730C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FFCAE73-9D12-7A4C-93C1-2D61E6FBC2B8}"/>
+  <xr:revisionPtr revIDLastSave="414" documentId="8_{3AB129F9-6C21-034E-B68D-3118804A730C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C9DCC32-64E5-B249-830E-0A00328045DA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" activeTab="1" xr2:uid="{648EA1FE-8C1C-FB4A-A645-0D83DAA06A0B}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{648EA1FE-8C1C-FB4A-A645-0D83DAA06A0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Python" sheetId="1" r:id="rId1"/>
@@ -165,11 +165,6 @@
     <t>Degree was not able to be scheduled in 2 years</t>
   </si>
   <si>
-    <t>Degree successfully scheduled in 4 years (8 semesters)
-num_semesters: 8
-num_years: 4.0</t>
-  </si>
-  <si>
     <t>First Year Taken</t>
   </si>
   <si>
@@ -250,21 +245,6 @@
   </si>
   <si>
     <t>Details</t>
-  </si>
-  <si>
-    <t>Degree successfully scheduled in 3 years (6 semesters)
-num_semesters: 6
-num_years: 3.0</t>
-  </si>
-  <si>
-    <t>Degree successfully scheduled in 2 years (4 semesters)
-num_semesters: 4
-num_years: 2.0</t>
-  </si>
-  <si>
-    <t>Degree successfully scheduled in 1 years (2 semesters)
-num_semesters: 2
-num_years: 1.0</t>
   </si>
   <si>
     <t>y</t>
@@ -343,11 +323,6 @@
     <t>Degree was not able to be scheduled in 10 years</t>
   </si>
   <si>
-    <t>Degree successfully scheduled in 3.0 years (6 semesters)
-num_semesters: 6
-num_years: 3.0</t>
-  </si>
-  <si>
     <t>Full Options + Cognate II
 Different options</t>
   </si>
@@ -380,11 +355,6 @@
   </si>
   <si>
     <t>Actually 9 years/18 semesters. This makes sense since there is not necessarily an equal number of fall/winter courses</t>
-  </si>
-  <si>
-    <t>Degree successfully scheduled in 9.0 years (18 semesters)
-num_semesters: 18
-num_years: 9.0</t>
   </si>
   <si>
     <t>Full Options + Cognate III
@@ -420,16 +390,6 @@
                 "MATH2311",
                 "MATH3101"
         ],</t>
-  </si>
-  <si>
-    <t>Degree successfully scheduled in 4.0 years (8 semesters)
-num_semesters: 8
-num_years: 4.0</t>
-  </si>
-  <si>
-    <t>Degree successfully scheduled in 5.0 years (10 semesters)
-num_semesters: 10
-num_years: 5.0</t>
   </si>
   <si>
     <t>Python Test Plan</t>
@@ -828,13 +788,46 @@
     <t>*note that test # might be different than order ran from tests.pl</t>
   </si>
   <si>
-    <t>*note that test # might be different than order ran from run_tests.py</t>
-  </si>
-  <si>
     <t>run tests (from root folder/parent folder of run_tests.py): "python3 run_tests.py"</t>
   </si>
   <si>
     <t>run tests (from prolog folder): "swipl tests.pl" -&gt; "run_tests."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree successfully scheduled in 4 years (8 semesters)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree successfully scheduled in 3 years (6 semesters)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree successfully scheduled in 2 years (4 semesters)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree successfully scheduled in 1 years (2 semesters)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree successfully scheduled in 3.0 years (6 semesters)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree successfully scheduled in 4.0 years (8 semesters)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree successfully scheduled in 5.0 years (10 semesters)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Degree successfully scheduled in 9.0 years (18 semesters)
+</t>
+  </si>
+  <si>
+    <t>*note that test # may different than order ran from run_tests.py
+run_tests is grouped by 'Reason'</t>
   </si>
 </sst>
 </file>
@@ -1340,11 +1333,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15EE35DF-1E31-B34F-BCFF-1FD3BCC0EA75}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1364,21 +1357,21 @@
     <row r="1" spans="1:9" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.35">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" s="10" customFormat="1" ht="37" x14ac:dyDescent="0.35">
       <c r="A2" s="8"/>
       <c r="B2" s="9"/>
-      <c r="G2" s="10" t="s">
-        <v>146</v>
+      <c r="G2" s="1" t="s">
+        <v>148</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -1412,7 +1405,7 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1439,7 +1432,7 @@
         <v>31</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1457,7 +1450,7 @@
         <v>2.json</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
@@ -1466,7 +1459,7 @@
         <v>31</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1493,7 +1486,7 @@
         <v>31</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1520,7 +1513,7 @@
         <v>31</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1547,7 +1540,7 @@
         <v>33</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1574,7 +1567,7 @@
         <v>33</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1601,7 +1594,7 @@
         <v>34</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -1625,10 +1618,10 @@
         <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1652,10 +1645,10 @@
         <v>17</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -1679,10 +1672,10 @@
         <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -1690,26 +1683,26 @@
         <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>11.json</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>54</v>
+        <v>141</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="170" x14ac:dyDescent="0.2">
@@ -1717,26 +1710,26 @@
         <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>12.json</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>55</v>
+        <v>142</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="238" x14ac:dyDescent="0.2">
@@ -1744,26 +1737,26 @@
         <v>13</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>13.json</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>13.json</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>56</v>
+        <v>143</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -1771,26 +1764,26 @@
         <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>14.json</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -1798,29 +1791,29 @@
         <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>15.json</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -1828,29 +1821,29 @@
         <v>16</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>16.json</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="170" x14ac:dyDescent="0.2">
@@ -1858,26 +1851,26 @@
         <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>17.json</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -1885,26 +1878,26 @@
         <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>18.json</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>68</v>
+        <v>144</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="306" x14ac:dyDescent="0.2">
@@ -1912,26 +1905,26 @@
         <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>19.json</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>35</v>
+        <v>140</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="170" x14ac:dyDescent="0.2">
@@ -1939,29 +1932,29 @@
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>20.json</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="119" x14ac:dyDescent="0.2">
@@ -1969,26 +1962,26 @@
         <v>21</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>21.json</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>87</v>
+        <v>146</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -1996,29 +1989,29 @@
         <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>22.json</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>22.json</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="G26" s="3" t="s">
-        <v>79</v>
+        <v>147</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2026,26 +2019,26 @@
         <v>23</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>23.json</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -2053,26 +2046,26 @@
         <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D28" s="2" t="str">
         <f t="shared" si="0"/>
         <v>24.json</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -2080,26 +2073,26 @@
         <v>25</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D29" s="2" t="str">
         <f t="shared" si="0"/>
         <v>25.json</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -2107,26 +2100,26 @@
         <v>26</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D30" s="2" t="str">
         <f t="shared" si="0"/>
         <v>26.json</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="187" x14ac:dyDescent="0.2">
@@ -2134,26 +2127,26 @@
         <v>27</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D31" s="2" t="str">
         <f t="shared" ref="D31" si="1">CONCATENATE(A31,".json")</f>
         <v>27.json</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2173,8 +2166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0408BD7-DCFB-044D-9C76-99080A8D7D40}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="2" ySplit="4" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
@@ -2197,13 +2190,13 @@
     <row r="1" spans="1:9" s="10" customFormat="1" ht="32" x14ac:dyDescent="0.35">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -2211,7 +2204,7 @@
       <c r="A2" s="5"/>
       <c r="B2" s="2"/>
       <c r="G2" s="10" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2244,7 +2237,7 @@
         <v>32</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2262,16 +2255,16 @@
         <v>1.json</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2289,16 +2282,16 @@
         <v>2.json</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2316,16 +2309,16 @@
         <v>3.json</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2343,16 +2336,16 @@
         <v>4.json</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2370,16 +2363,16 @@
         <v>5.json</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2397,16 +2390,16 @@
         <v>6.json</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2424,16 +2417,16 @@
         <v>7.json</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="272" x14ac:dyDescent="0.2">
@@ -2451,16 +2444,16 @@
         <v>8.json</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="272" x14ac:dyDescent="0.2">
@@ -2478,16 +2471,16 @@
         <v>9.json</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="272" x14ac:dyDescent="0.2">
@@ -2505,16 +2498,16 @@
         <v>10.json</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="204" x14ac:dyDescent="0.2">
@@ -2522,26 +2515,26 @@
         <v>11</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>11.json</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="170" x14ac:dyDescent="0.2">
@@ -2549,26 +2542,26 @@
         <v>12</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>12.json</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="238" x14ac:dyDescent="0.2">
@@ -2576,26 +2569,26 @@
         <v>13</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>13.json</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -2603,29 +2596,29 @@
         <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D18" s="2" t="str">
         <f t="shared" si="0"/>
         <v>14.json</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -2633,26 +2626,26 @@
         <v>15</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>15.json</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="119" x14ac:dyDescent="0.2">
@@ -2660,26 +2653,26 @@
         <v>16</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>16.json</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="372" x14ac:dyDescent="0.2">
@@ -2687,26 +2680,26 @@
         <v>17</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>17.json</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="372" x14ac:dyDescent="0.2">
@@ -2714,26 +2707,26 @@
         <v>18</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="2" t="str">
         <f t="shared" ref="D22:D25" si="1">CONCATENATE(A22,".json")</f>
         <v>18.json</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -2741,26 +2734,26 @@
         <v>19</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D23" s="2" t="str">
         <f t="shared" si="1"/>
         <v>19.json</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -2768,26 +2761,26 @@
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D24" s="2" t="str">
         <f t="shared" si="1"/>
         <v>20.json</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="170" x14ac:dyDescent="0.2">
@@ -2795,26 +2788,26 @@
         <v>21</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D25" s="2" t="str">
         <f t="shared" si="1"/>
         <v>21.json</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="272" x14ac:dyDescent="0.2">
@@ -2822,26 +2815,26 @@
         <v>22</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>22.json</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>22.json</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="G26" s="3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -2849,29 +2842,29 @@
         <v>23</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D27" s="2" t="str">
         <f>CONCATENATE(A27,".json")</f>
         <v>23.json</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>